<commit_message>
Add change password feature to Admin Panel
Store the parent approval password in data.config (default '1234') so it
persists across restarts. Add a Change Password widget in the Admin Panel
with current/new/confirm inputs and validation. Update Dashboard and
GoalRoom to read the password from config instead of using a hardcoded value.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/goal_app_data.xlsx
+++ b/goal_app_data.xlsx
@@ -506,6 +506,7 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
   </ignoredErrors>
@@ -586,6 +587,7 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
@@ -594,7 +596,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -607,16 +609,25 @@
         <v>Jackson Goal</v>
       </c>
       <c r="C1" t="str">
+        <v>Jackson Goal Credits</v>
+      </c>
+      <c r="D1" t="str">
         <v>Natalie</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>Natalie Goal</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
+        <v>Natalie Goal Credits</v>
+      </c>
+      <c r="G1" t="str">
         <v>Brooke</v>
       </c>
-      <c r="F1" t="str">
+      <c r="H1" t="str">
         <v>Brooke Goal</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Brooke Goal Credits</v>
       </c>
     </row>
     <row r="2">
@@ -624,31 +635,99 @@
         <v>play baseball game</v>
       </c>
       <c r="B2" t="str">
+        <v>Hit Baseball Over Infeed</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="str">
+        <v>play softball game</v>
+      </c>
+      <c r="E2" t="str">
         <v>Get a Out</v>
       </c>
-      <c r="C2" t="str">
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" t="str">
         <v>play softball game</v>
       </c>
-      <c r="D2" t="str">
+      <c r="H2" t="str">
+        <v>Hit a Pitch from a Kid</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
         <v>Get a Out</v>
       </c>
-      <c r="E2" t="str">
-        <v>play softball game</v>
-      </c>
-      <c r="F2" t="str">
-        <v>Hit Pitch from Kid</v>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <v>Hit a Double</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <v>Get a Out</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <v/>
+      </c>
+      <c r="C4" t="str">
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v>Go a Whole Week Without Yelling at Mom</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
+      <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -699,7 +778,7 @@
         <v>yes</v>
       </c>
       <c r="C2" t="str">
-        <v>Breakfast Oats</v>
+        <v>Doughnuts</v>
       </c>
       <c r="D2" t="str">
         <v>yes</v>
@@ -723,7 +802,7 @@
         <v>yes</v>
       </c>
       <c r="K2" t="str">
-        <v>Cheese stick</v>
+        <v>Fruit Rolls</v>
       </c>
       <c r="L2" t="str">
         <v>yes</v>
@@ -737,7 +816,7 @@
         <v>yes</v>
       </c>
       <c r="C3" t="str">
-        <v>Doughnuts</v>
+        <v>French Toast</v>
       </c>
       <c r="D3" t="str">
         <v>yes</v>
@@ -761,7 +840,7 @@
         <v>yes</v>
       </c>
       <c r="K3" t="str">
-        <v>Fruit Rolls</v>
+        <v>Granola bar</v>
       </c>
       <c r="L3" t="str">
         <v>yes</v>
@@ -775,7 +854,7 @@
         <v>yes</v>
       </c>
       <c r="C4" t="str">
-        <v>French Toast</v>
+        <v>Pancakes</v>
       </c>
       <c r="D4" t="str">
         <v>yes</v>
@@ -799,7 +878,7 @@
         <v>yes</v>
       </c>
       <c r="K4" t="str">
-        <v>Granola bar</v>
+        <v>Apple Sauce Pouch</v>
       </c>
       <c r="L4" t="str">
         <v>yes</v>
@@ -813,7 +892,7 @@
         <v>yes</v>
       </c>
       <c r="C5" t="str">
-        <v>Pancakes</v>
+        <v>Waffles</v>
       </c>
       <c r="D5" t="str">
         <v>yes</v>
@@ -837,7 +916,7 @@
         <v>yes</v>
       </c>
       <c r="K5" t="str">
-        <v>Apple Sauce Pouch</v>
+        <v>Pretzels</v>
       </c>
       <c r="L5" t="str">
         <v>yes</v>
@@ -851,10 +930,10 @@
         <v>yes</v>
       </c>
       <c r="C6" t="str">
-        <v>Waffles</v>
+        <v/>
       </c>
       <c r="D6" t="str">
-        <v>yes</v>
+        <v/>
       </c>
       <c r="E6" t="str">
         <v>Peanut Butter and Jelly</v>
@@ -875,7 +954,7 @@
         <v>yes</v>
       </c>
       <c r="K6" t="str">
-        <v>Pretzels</v>
+        <v>Ritz Crackers</v>
       </c>
       <c r="L6" t="str">
         <v>yes</v>
@@ -913,10 +992,10 @@
         <v>yes</v>
       </c>
       <c r="K7" t="str">
-        <v/>
+        <v>Doritos</v>
       </c>
       <c r="L7" t="str">
-        <v/>
+        <v>yes</v>
       </c>
     </row>
     <row r="8">
@@ -951,10 +1030,10 @@
         <v>yes</v>
       </c>
       <c r="K8" t="str">
-        <v/>
+        <v>Sun Chips</v>
       </c>
       <c r="L8" t="str">
-        <v/>
+        <v>yes</v>
       </c>
     </row>
     <row r="9">
@@ -1185,9 +1264,85 @@
         <v/>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Keish</v>
+      </c>
+      <c r="B15" t="str">
+        <v>yes</v>
+      </c>
+      <c r="C15" t="str">
+        <v/>
+      </c>
+      <c r="D15" t="str">
+        <v/>
+      </c>
+      <c r="E15" t="str">
+        <v/>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <v/>
+      </c>
+      <c r="H15" t="str">
+        <v/>
+      </c>
+      <c r="I15" t="str">
+        <v/>
+      </c>
+      <c r="J15" t="str">
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <v/>
+      </c>
+      <c r="L15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Breakfast Oats</v>
+      </c>
+      <c r="B16" t="str">
+        <v>yes</v>
+      </c>
+      <c r="C16" t="str">
+        <v/>
+      </c>
+      <c r="D16" t="str">
+        <v/>
+      </c>
+      <c r="E16" t="str">
+        <v/>
+      </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <v/>
+      </c>
+      <c r="H16" t="str">
+        <v/>
+      </c>
+      <c r="I16" t="str">
+        <v/>
+      </c>
+      <c r="J16" t="str">
+        <v/>
+      </c>
+      <c r="K16" t="str">
+        <v/>
+      </c>
+      <c r="L16" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L16"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1420,6 +1575,7 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:F11"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Rename View Selections to View Status and make mode-aware
- Button and header text changed to VIEW STATUS
- Tasks now filtered to current quest mode only (no stale morning tasks on weekend)
- Food section only shown during morning mode
- Goals only shown if completed today (checked against goal_log)
- Fixed crash rendering goal objects as React children

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/goal_app_data.xlsx
+++ b/goal_app_data.xlsx
@@ -506,6 +506,7 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
   </ignoredErrors>
@@ -586,6 +587,7 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
@@ -716,6 +718,7 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
   </ignoredErrors>
@@ -768,8 +771,14 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="str">
+        <v>Oatmeal</v>
+      </c>
       <c r="B2" t="str">
         <v>yes</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Doughnuts</v>
       </c>
       <c r="D2" t="str">
         <v>yes</v>
@@ -800,6 +809,9 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="str">
+        <v>Breakfast Oats</v>
+      </c>
       <c r="B3" t="str">
         <v>yes</v>
       </c>
@@ -835,6 +847,9 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="str">
+        <v>Eggs</v>
+      </c>
       <c r="B4" t="str">
         <v>yes</v>
       </c>

</xml_diff>